<commit_message>
Modified dummy lifetime value to 2.5 years to make the graphs make more sense
</commit_message>
<xml_diff>
--- a/docs/Files/Li_Lifetime_US.xlsx
+++ b/docs/Files/Li_Lifetime_US.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvend\Documents\CodeProjects\ODYM\docs\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28DF2C7-9F90-43C1-8D1B-9F19402E2A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D131896A-3669-4CF7-AFA6-B580BFF7DDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9456" yWindow="420" windowWidth="13584" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Average_Lifetime" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -366,7 +366,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>